<commit_message>
finish air temperature script
</commit_message>
<xml_diff>
--- a/outputs/rainfall/2025/rainfall_monthly-percentiles.xlsx
+++ b/outputs/rainfall/2025/rainfall_monthly-percentiles.xlsx
@@ -619,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="N3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O3">
         <v>6</v>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -865,7 +865,7 @@
         <v>5</v>
       </c>
       <c r="K8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -1324,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="K17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L17">
         <v>3</v>

</xml_diff>